<commit_message>
Atualização Atividade 2 - Lista de variáveis
Listagem das classes ReciboControllerTeste e RaciboDAOTeste.
</commit_message>
<xml_diff>
--- a/Atividade 2 - Lista de variáveis _C.xlsx
+++ b/Atividade 2 - Lista de variáveis _C.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="457">
   <si>
     <t>Class</t>
   </si>
@@ -1769,6 +1769,297 @@
   </si>
   <si>
     <t>Used to receive the result from the search for a receipt on DB</t>
+  </si>
+  <si>
+    <t>AgendaControllerTeste.java</t>
+  </si>
+  <si>
+    <t>PhonebookControllerTest.java</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instance of class 'Agenda.java' used to test </t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Initialize the atributes of 'contact'(refers to instance above)</t>
+    </r>
+  </si>
+  <si>
+    <t>barberException</t>
+  </si>
+  <si>
+    <t>contactController</t>
+  </si>
+  <si>
+    <t>Instantiated to get access to the methods of class 'AgendaController'</t>
+  </si>
+  <si>
+    <t>getInstanceDeAgendaControllerDeveRetornarInstanciaCorrente</t>
+  </si>
+  <si>
+    <t>inserirDeAgendaControllerDeveEnviarUm</t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test if a inclusion of a contact was made right (check the return of method 'inserir')</t>
+    </r>
+  </si>
+  <si>
+    <t>excluirDeAgendaControllerDeveEnviarUmaAgenda</t>
+  </si>
+  <si>
+    <t>includeContactMethodTest</t>
+  </si>
+  <si>
+    <t>deleteContactMethodTest</t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test if a exclusion of a contact was made right (check the return of method 'excluir')</t>
+    </r>
+  </si>
+  <si>
+    <t>alterarDeAgendaControllerDeveEnviarUmaAgendaAlterada</t>
+  </si>
+  <si>
+    <t>modifyContactMethodTest</t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test if a modification of a contact was made right (check the return of method 'alterar')</t>
+    </r>
+  </si>
+  <si>
+    <t>inserirAgendaNaoPodePassarAgendaNullo</t>
+  </si>
+  <si>
+    <t>includeContactMethodTestForNullArgument</t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test if the method 'inserir' don't accept null argument</t>
+    </r>
+  </si>
+  <si>
+    <t>excluirAgendaNaoPodePassarAgendaNullo</t>
+  </si>
+  <si>
+    <t>deleteContactMethodTestForNullArgument</t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test if the method 'excluir' don't accept null argument</t>
+    </r>
+  </si>
+  <si>
+    <t>alterarAgendaNaoPodePassarAgendaNullo</t>
+  </si>
+  <si>
+    <t>modifyContactMethodTestForNullArgument</t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test if the method 'alterar' don't accept null argument</t>
+    </r>
+  </si>
+  <si>
+    <t>mostrarContatosDeAgendaControllerDeveMostrarUmContato</t>
+  </si>
+  <si>
+    <t>showRegisteredContactsTest</t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test the method 'mostrarContatosCadastrados'</t>
+    </r>
+  </si>
+  <si>
+    <t>queryForContactsResult</t>
+  </si>
+  <si>
+    <t>pesquisarPorNomeDeAgendaControllerDeveMostrarUmContato</t>
+  </si>
+  <si>
+    <t>searchContactsByNameTest</t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test the method 'pesquisaPorNome'</t>
+    </r>
+  </si>
+  <si>
+    <t>Used to receive the result from the search for contacts on DB</t>
+  </si>
+  <si>
+    <t>pesquisarPorTelefoneDeAgendaControllerDeveMostrarUmContato</t>
+  </si>
+  <si>
+    <t>searchContactsByPhoneTest</t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test the method 'pesquisaPorTelefone'</t>
+    </r>
+  </si>
+  <si>
+    <t>ReciboDAOTeste.java</t>
+  </si>
+  <si>
+    <t>ReceiptDAOTest.java</t>
+  </si>
+  <si>
+    <t>Instance variable used to test</t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Initialize the atributes of 'report'(refers to instance above)</t>
+    </r>
+  </si>
+  <si>
+    <t>reportException</t>
+  </si>
+  <si>
+    <t>reciboDAO</t>
+  </si>
+  <si>
+    <t>receipt</t>
+  </si>
+  <si>
+    <t>pesquisarPorDataEBArbeiroDAODeveMostrarUmRecibo</t>
+  </si>
+  <si>
+    <t>Instantiated to get access to the method 'pesquisarServicosDoBarbeiro' of class 'ReciboDAO.java'</t>
+  </si>
+  <si>
+    <t>searchBarberServicesMethodTest</t>
+  </si>
+  <si>
+    <r>
+      <t>Method name -&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test the method 'pesquisaSerivcosDoBarbeiro' (if returns the right services of a barber)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2357,13 +2648,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2384,19 +2672,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2417,7 +2708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2426,7 +2717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2435,10 +2726,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2737,7 +3028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView topLeftCell="C32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
@@ -2775,10 +3066,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -2798,8 +3089,8 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="28"/>
-      <c r="B3" s="25"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="7" t="s">
         <v>196</v>
       </c>
@@ -2817,12 +3108,12 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="28"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="21" t="s">
+      <c r="A4" s="27"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
@@ -2836,10 +3127,10 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="28"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="5" t="s">
         <v>201</v>
       </c>
@@ -2851,10 +3142,10 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="28"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
       <c r="E6" s="5" t="s">
         <v>204</v>
       </c>
@@ -2866,10 +3157,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="28"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="5" t="s">
         <v>206</v>
       </c>
@@ -2881,10 +3172,10 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="28"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="5" t="s">
         <v>197</v>
       </c>
@@ -2896,10 +3187,10 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="28"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="5" t="s">
         <v>210</v>
       </c>
@@ -2911,10 +3202,10 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="29"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="5" t="s">
         <v>214</v>
       </c>
@@ -2935,10 +3226,10 @@
       <c r="G11" s="16"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>289</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -2958,12 +3249,12 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="28"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="32" t="s">
+      <c r="A13" s="27"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -2977,10 +3268,10 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="28"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="5" t="s">
         <v>233</v>
       </c>
@@ -2992,12 +3283,12 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="28"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="21" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="30" t="s">
         <v>293</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="30" t="s">
         <v>294</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -3011,10 +3302,10 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="28"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="5" t="s">
         <v>295</v>
       </c>
@@ -3026,10 +3317,10 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="28"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="5" t="s">
         <v>299</v>
       </c>
@@ -3041,10 +3332,10 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="28"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="5" t="s">
         <v>304</v>
       </c>
@@ -3056,10 +3347,10 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="28"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="5" t="s">
         <v>305</v>
       </c>
@@ -3071,10 +3362,10 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="28"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="5" t="s">
         <v>310</v>
       </c>
@@ -3086,10 +3377,10 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="28"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="5" t="s">
         <v>311</v>
       </c>
@@ -3101,10 +3392,10 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="28"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="5" t="s">
         <v>314</v>
       </c>
@@ -3116,10 +3407,10 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="28"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="5" t="s">
         <v>317</v>
       </c>
@@ -3131,10 +3422,10 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="28"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="5" t="s">
         <v>320</v>
       </c>
@@ -3146,10 +3437,10 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="28"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
       <c r="E25" s="5" t="s">
         <v>322</v>
       </c>
@@ -3161,10 +3452,10 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="28"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
       <c r="E26" s="5" t="s">
         <v>325</v>
       </c>
@@ -3176,10 +3467,10 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="29"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
       <c r="E27" s="5" t="s">
         <v>233</v>
       </c>
@@ -3200,16 +3491,16 @@
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>329</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="23" t="s">
         <v>330</v>
       </c>
-      <c r="C29" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="32" t="s">
+      <c r="C29" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -3223,10 +3514,10 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="28"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
       <c r="E30" s="5" t="s">
         <v>331</v>
       </c>
@@ -3238,10 +3529,10 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="28"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="5" t="s">
         <v>332</v>
       </c>
@@ -3253,10 +3544,10 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="28"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
       <c r="E32" s="5" t="s">
         <v>333</v>
       </c>
@@ -3268,10 +3559,10 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="28"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="5" t="s">
         <v>19</v>
       </c>
@@ -3283,12 +3574,12 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="28"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="32" t="s">
+      <c r="A34" s="27"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="D34" s="32" t="s">
+      <c r="D34" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E34" s="5" t="s">
@@ -3302,10 +3593,10 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="28"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
       <c r="E35" s="5" t="s">
         <v>233</v>
       </c>
@@ -3317,12 +3608,12 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="28"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="21" t="s">
+      <c r="A36" s="27"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="30" t="s">
         <v>344</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="30" t="s">
         <v>345</v>
       </c>
       <c r="E36" s="9" t="s">
@@ -3336,10 +3627,10 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="28"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
       <c r="E37" s="5" t="s">
         <v>346</v>
       </c>
@@ -3351,10 +3642,10 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="28"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
       <c r="E38" s="5" t="s">
         <v>347</v>
       </c>
@@ -3366,10 +3657,10 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="28"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
       <c r="E39" s="5" t="s">
         <v>348</v>
       </c>
@@ -3381,10 +3672,10 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="28"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
       <c r="E40" s="5" t="s">
         <v>355</v>
       </c>
@@ -3396,10 +3687,10 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="28"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
       <c r="E41" s="5" t="s">
         <v>358</v>
       </c>
@@ -3411,10 +3702,10 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="28"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
       <c r="E42" s="5" t="s">
         <v>76</v>
       </c>
@@ -3426,10 +3717,10 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="28"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
       <c r="E43" s="5" t="s">
         <v>233</v>
       </c>
@@ -3441,10 +3732,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="28"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
       <c r="E44" s="5" t="s">
         <v>233</v>
       </c>
@@ -3456,10 +3747,10 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="28"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
       <c r="E45" s="5" t="s">
         <v>367</v>
       </c>
@@ -3471,10 +3762,10 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="28"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
       <c r="E46" s="5" t="s">
         <v>374</v>
       </c>
@@ -3486,10 +3777,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="28"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
       <c r="E47" s="5" t="s">
         <v>376</v>
       </c>
@@ -3501,10 +3792,10 @@
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="28"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
       <c r="E48" s="5" t="s">
         <v>377</v>
       </c>
@@ -3516,10 +3807,10 @@
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="28"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="5" t="s">
         <v>378</v>
       </c>
@@ -3531,10 +3822,10 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="28"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
       <c r="E50" s="5" t="s">
         <v>379</v>
       </c>
@@ -3546,10 +3837,10 @@
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="28"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
       <c r="E51" s="5" t="s">
         <v>317</v>
       </c>
@@ -3561,10 +3852,10 @@
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="28"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
+      <c r="A52" s="27"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
       <c r="E52" s="5" t="s">
         <v>320</v>
       </c>
@@ -3576,12 +3867,12 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="28"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="32" t="s">
+      <c r="A53" s="27"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="21" t="s">
         <v>381</v>
       </c>
-      <c r="D53" s="32" t="s">
+      <c r="D53" s="21" t="s">
         <v>382</v>
       </c>
       <c r="E53" s="5" t="s">
@@ -3595,10 +3886,10 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="29"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
       <c r="E54" s="5" t="s">
         <v>383</v>
       </c>
@@ -3899,6 +4190,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D15:D27"/>
+    <mergeCell ref="C15:C27"/>
+    <mergeCell ref="B12:B27"/>
+    <mergeCell ref="A12:A27"/>
+    <mergeCell ref="D4:D10"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="D53:D54"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="B29:B54"/>
@@ -3909,16 +4210,6 @@
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="D36:D52"/>
     <mergeCell ref="C36:C52"/>
-    <mergeCell ref="D15:D27"/>
-    <mergeCell ref="C15:C27"/>
-    <mergeCell ref="B12:B27"/>
-    <mergeCell ref="A12:A27"/>
-    <mergeCell ref="D4:D10"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3929,7 +4220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
@@ -3966,10 +4257,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>88</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -3989,10 +4280,10 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="28"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="5" t="s">
         <v>90</v>
       </c>
@@ -4004,10 +4295,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="28"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="5" t="s">
         <v>91</v>
       </c>
@@ -4019,10 +4310,10 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="28"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
@@ -4034,10 +4325,10 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="28"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="5" t="s">
         <v>92</v>
       </c>
@@ -4049,10 +4340,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="28"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="5" t="s">
         <v>93</v>
       </c>
@@ -4064,10 +4355,10 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="28"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="5" t="s">
         <v>94</v>
       </c>
@@ -4079,10 +4370,10 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="28"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="5" t="s">
         <v>95</v>
       </c>
@@ -4094,12 +4385,12 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="28"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="21" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="30" t="s">
         <v>109</v>
       </c>
       <c r="E10" s="9" t="s">
@@ -4113,10 +4404,10 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="28"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="5" t="s">
         <v>89</v>
       </c>
@@ -4128,10 +4419,10 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="28"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
       <c r="E12" s="5" t="s">
         <v>90</v>
       </c>
@@ -4143,10 +4434,10 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="28"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
       <c r="E13" s="5" t="s">
         <v>91</v>
       </c>
@@ -4158,10 +4449,10 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="28"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
       <c r="E14" s="5" t="s">
         <v>15</v>
       </c>
@@ -4173,8 +4464,8 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="28"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="10" t="s">
         <v>108</v>
       </c>
@@ -4192,8 +4483,8 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="28"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="7" t="s">
         <v>111</v>
       </c>
@@ -4211,12 +4502,12 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="28"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="32" t="s">
+      <c r="A17" s="27"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="21" t="s">
         <v>115</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -4230,10 +4521,10 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="28"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="5" t="s">
         <v>117</v>
       </c>
@@ -4245,10 +4536,10 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="28"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="5" t="s">
         <v>119</v>
       </c>
@@ -4260,10 +4551,10 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="28"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="5" t="s">
         <v>122</v>
       </c>
@@ -4275,10 +4566,10 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="28"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
       <c r="E21" s="5" t="s">
         <v>124</v>
       </c>
@@ -4290,8 +4581,8 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="28"/>
-      <c r="B22" s="25"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="7" t="s">
         <v>127</v>
       </c>
@@ -4309,12 +4600,12 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="28"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="32" t="s">
+      <c r="A23" s="27"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="21" t="s">
         <v>131</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -4328,10 +4619,10 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="28"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="5" t="s">
         <v>117</v>
       </c>
@@ -4343,10 +4634,10 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="28"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="5" t="s">
         <v>119</v>
       </c>
@@ -4358,10 +4649,10 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="28"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="5" t="s">
         <v>122</v>
       </c>
@@ -4373,10 +4664,10 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="28"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="5" t="s">
         <v>124</v>
       </c>
@@ -4388,8 +4679,8 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="28"/>
-      <c r="B28" s="25"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="7" t="s">
         <v>136</v>
       </c>
@@ -4407,8 +4698,8 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="28"/>
-      <c r="B29" s="25"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="7" t="s">
         <v>137</v>
       </c>
@@ -4426,8 +4717,8 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="28"/>
-      <c r="B30" s="25"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="7" t="s">
         <v>142</v>
       </c>
@@ -4445,8 +4736,8 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="28"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="7" t="s">
         <v>143</v>
       </c>
@@ -4464,12 +4755,12 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="28"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="32" t="s">
+      <c r="A32" s="27"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D32" s="21" t="s">
         <v>149</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -4483,10 +4774,10 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="28"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="5" t="s">
         <v>151</v>
       </c>
@@ -4498,10 +4789,10 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="28"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
       <c r="E34" s="5" t="s">
         <v>117</v>
       </c>
@@ -4513,10 +4804,10 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="28"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
       <c r="E35" s="5" t="s">
         <v>124</v>
       </c>
@@ -4528,10 +4819,10 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="28"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
       <c r="E36" s="5" t="s">
         <v>122</v>
       </c>
@@ -4543,10 +4834,10 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="29"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="5" t="s">
         <v>154</v>
       </c>
@@ -4567,16 +4858,16 @@
       <c r="G38" s="16"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="C39" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="32" t="s">
+      <c r="C39" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E39" s="5" t="s">
@@ -4590,10 +4881,10 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="28"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
       <c r="E40" s="5" t="s">
         <v>161</v>
       </c>
@@ -4605,10 +4896,10 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="28"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
       <c r="E41" s="5" t="s">
         <v>162</v>
       </c>
@@ -4620,10 +4911,10 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="28"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
       <c r="E42" s="5" t="s">
         <v>163</v>
       </c>
@@ -4635,10 +4926,10 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="28"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
       <c r="E43" s="5" t="s">
         <v>164</v>
       </c>
@@ -4650,10 +4941,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="28"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="5" t="s">
         <v>165</v>
       </c>
@@ -4665,8 +4956,8 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="28"/>
-      <c r="B45" s="25"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="10" t="s">
         <v>157</v>
       </c>
@@ -4684,8 +4975,8 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="28"/>
-      <c r="B46" s="25"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="24"/>
       <c r="C46" s="5" t="s">
         <v>175</v>
       </c>
@@ -4703,8 +4994,8 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="28"/>
-      <c r="B47" s="25"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="24"/>
       <c r="C47" s="5" t="s">
         <v>176</v>
       </c>
@@ -4722,8 +5013,8 @@
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="28"/>
-      <c r="B48" s="25"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="24"/>
       <c r="C48" s="5" t="s">
         <v>177</v>
       </c>
@@ -4741,8 +5032,8 @@
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="28"/>
-      <c r="B49" s="25"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="24"/>
       <c r="C49" s="5" t="s">
         <v>184</v>
       </c>
@@ -4760,8 +5051,8 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="28"/>
-      <c r="B50" s="25"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="24"/>
       <c r="C50" s="5" t="s">
         <v>185</v>
       </c>
@@ -4779,8 +5070,8 @@
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="29"/>
-      <c r="B51" s="26"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="25"/>
       <c r="C51" s="5" t="s">
         <v>186</v>
       </c>
@@ -5055,7 +5346,7 @@
       <c r="A2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -5076,11 +5367,11 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="36"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="21" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -5095,9 +5386,9 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="36"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
@@ -5110,11 +5401,11 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="36"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="21" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -5129,9 +5420,9 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="36"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
@@ -5144,9 +5435,9 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="36"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="5" t="s">
         <v>15</v>
       </c>
@@ -5159,9 +5450,9 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="36"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
@@ -5174,11 +5465,11 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="36"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="32" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="21" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -5193,9 +5484,9 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="36"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="5" t="s">
         <v>15</v>
       </c>
@@ -5208,7 +5499,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="36"/>
-      <c r="B11" s="25"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="10" t="s">
         <v>39</v>
       </c>
@@ -5227,11 +5518,11 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="36"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="32" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -5246,9 +5537,9 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="36"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="11" t="s">
         <v>44</v>
       </c>
@@ -5261,11 +5552,11 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="36"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="32" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E14" s="12" t="s">
@@ -5280,9 +5571,9 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="37"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="5" t="s">
         <v>44</v>
       </c>
@@ -5470,7 +5761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -5530,10 +5821,10 @@
       <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -5553,8 +5844,8 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="28"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="10" t="s">
         <v>56</v>
       </c>
@@ -5572,8 +5863,8 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="28"/>
-      <c r="B6" s="25"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="7" t="s">
         <v>59</v>
       </c>
@@ -5591,12 +5882,12 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="28"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="32" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="21" t="s">
         <v>62</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -5610,10 +5901,10 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="28"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="5" t="s">
         <v>44</v>
       </c>
@@ -5625,12 +5916,12 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="28"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="32" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="21" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -5644,10 +5935,10 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="28"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="5" t="s">
         <v>44</v>
       </c>
@@ -5659,12 +5950,12 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="28"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="32" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -5678,10 +5969,10 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="28"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="5" t="s">
         <v>44</v>
       </c>
@@ -5693,10 +5984,10 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="28"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="5" t="s">
         <v>73</v>
       </c>
@@ -5708,10 +5999,10 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="28"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="5" t="s">
         <v>75</v>
       </c>
@@ -5723,10 +6014,10 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="28"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="5" t="s">
         <v>76</v>
       </c>
@@ -5738,12 +6029,12 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="28"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="32" t="s">
+      <c r="A16" s="27"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -5757,10 +6048,10 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="28"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="5" t="s">
         <v>79</v>
       </c>
@@ -5772,10 +6063,10 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="28"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="5" t="s">
         <v>73</v>
       </c>
@@ -5787,10 +6078,10 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="28"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="5" t="s">
         <v>75</v>
       </c>
@@ -5802,12 +6093,12 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="28"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="32" t="s">
+      <c r="A20" s="27"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="21" t="s">
         <v>81</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -5821,10 +6112,10 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="28"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="11" t="s">
         <v>44</v>
       </c>
@@ -5836,10 +6127,10 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="28"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="5" t="s">
         <v>73</v>
       </c>
@@ -5851,10 +6142,10 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="29"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="5" t="s">
         <v>76</v>
       </c>
@@ -6094,10 +6385,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:G44"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6134,10 +6425,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="47" t="s">
         <v>217</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="48" t="s">
         <v>218</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -6159,10 +6450,10 @@
     <row r="3" spans="1:7">
       <c r="A3" s="45"/>
       <c r="B3" s="42"/>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="21" t="s">
         <v>221</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -6178,8 +6469,8 @@
     <row r="4" spans="1:7">
       <c r="A4" s="45"/>
       <c r="B4" s="42"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="5" t="s">
         <v>223</v>
       </c>
@@ -6250,10 +6541,10 @@
     <row r="8" spans="1:7">
       <c r="A8" s="45"/>
       <c r="B8" s="42"/>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="21" t="s">
         <v>241</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -6269,8 +6560,8 @@
     <row r="9" spans="1:7">
       <c r="A9" s="45"/>
       <c r="B9" s="42"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="5" t="s">
         <v>233</v>
       </c>
@@ -6341,10 +6632,10 @@
     <row r="13" spans="1:7">
       <c r="A13" s="45"/>
       <c r="B13" s="42"/>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="21" t="s">
         <v>252</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -6360,8 +6651,8 @@
     <row r="14" spans="1:7">
       <c r="A14" s="45"/>
       <c r="B14" s="42"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="5" t="s">
         <v>233</v>
       </c>
@@ -6432,10 +6723,10 @@
     <row r="18" spans="1:7">
       <c r="A18" s="45"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="21" t="s">
         <v>263</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -6451,8 +6742,8 @@
     <row r="19" spans="1:7">
       <c r="A19" s="45"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="5" t="s">
         <v>233</v>
       </c>
@@ -6466,10 +6757,10 @@
     <row r="20" spans="1:7">
       <c r="A20" s="45"/>
       <c r="B20" s="42"/>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="21" t="s">
         <v>266</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -6485,8 +6776,8 @@
     <row r="21" spans="1:7">
       <c r="A21" s="45"/>
       <c r="B21" s="42"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="5" t="s">
         <v>233</v>
       </c>
@@ -6500,8 +6791,8 @@
     <row r="22" spans="1:7">
       <c r="A22" s="45"/>
       <c r="B22" s="42"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="5" t="s">
         <v>233</v>
       </c>
@@ -6515,10 +6806,10 @@
     <row r="23" spans="1:7">
       <c r="A23" s="45"/>
       <c r="B23" s="42"/>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="21" t="s">
         <v>274</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -6534,8 +6825,8 @@
     <row r="24" spans="1:7">
       <c r="A24" s="45"/>
       <c r="B24" s="42"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="5" t="s">
         <v>233</v>
       </c>
@@ -6549,8 +6840,8 @@
     <row r="25" spans="1:7">
       <c r="A25" s="45"/>
       <c r="B25" s="42"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="5" t="s">
         <v>233</v>
       </c>
@@ -6564,10 +6855,10 @@
     <row r="26" spans="1:7">
       <c r="A26" s="45"/>
       <c r="B26" s="42"/>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="21" t="s">
         <v>276</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="21" t="s">
         <v>277</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -6583,8 +6874,8 @@
     <row r="27" spans="1:7">
       <c r="A27" s="45"/>
       <c r="B27" s="42"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="5" t="s">
         <v>233</v>
       </c>
@@ -6598,8 +6889,8 @@
     <row r="28" spans="1:7">
       <c r="A28" s="45"/>
       <c r="B28" s="42"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="5" t="s">
         <v>233</v>
       </c>
@@ -6613,10 +6904,10 @@
     <row r="29" spans="1:7">
       <c r="A29" s="45"/>
       <c r="B29" s="42"/>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="D29" s="21" t="s">
         <v>280</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -6632,8 +6923,8 @@
     <row r="30" spans="1:7">
       <c r="A30" s="45"/>
       <c r="B30" s="42"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="5" t="s">
         <v>233</v>
       </c>
@@ -6647,10 +6938,10 @@
     <row r="31" spans="1:7">
       <c r="A31" s="45"/>
       <c r="B31" s="42"/>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="21" t="s">
         <v>283</v>
       </c>
       <c r="E31" s="5" t="s">
@@ -6666,8 +6957,8 @@
     <row r="32" spans="1:7">
       <c r="A32" s="45"/>
       <c r="B32" s="42"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
       <c r="E32" s="5" t="s">
         <v>233</v>
       </c>
@@ -6681,8 +6972,8 @@
     <row r="33" spans="1:7">
       <c r="A33" s="45"/>
       <c r="B33" s="42"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="5" t="s">
         <v>233</v>
       </c>
@@ -6722,10 +7013,10 @@
       <c r="G35" s="16"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="44" t="s">
         <v>386</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="41" t="s">
         <v>387</v>
       </c>
       <c r="C36" s="7" t="s">
@@ -6747,10 +7038,10 @@
     <row r="37" spans="1:7">
       <c r="A37" s="45"/>
       <c r="B37" s="42"/>
-      <c r="C37" s="32" t="s">
+      <c r="C37" s="21" t="s">
         <v>391</v>
       </c>
-      <c r="D37" s="32" t="s">
+      <c r="D37" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E37" s="5" t="s">
@@ -6766,8 +7057,8 @@
     <row r="38" spans="1:7">
       <c r="A38" s="45"/>
       <c r="B38" s="42"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="5" t="s">
         <v>233</v>
       </c>
@@ -6781,10 +7072,10 @@
     <row r="39" spans="1:7">
       <c r="A39" s="45"/>
       <c r="B39" s="42"/>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="21" t="s">
         <v>395</v>
       </c>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="21" t="s">
         <v>402</v>
       </c>
       <c r="E39" s="5" t="s">
@@ -6800,8 +7091,8 @@
     <row r="40" spans="1:7">
       <c r="A40" s="45"/>
       <c r="B40" s="42"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
       <c r="E40" s="5" t="s">
         <v>397</v>
       </c>
@@ -6815,10 +7106,10 @@
     <row r="41" spans="1:7">
       <c r="A41" s="45"/>
       <c r="B41" s="42"/>
-      <c r="C41" s="32" t="s">
+      <c r="C41" s="21" t="s">
         <v>400</v>
       </c>
-      <c r="D41" s="32" t="s">
+      <c r="D41" s="21" t="s">
         <v>403</v>
       </c>
       <c r="E41" s="5" t="s">
@@ -6834,8 +7125,8 @@
     <row r="42" spans="1:7">
       <c r="A42" s="45"/>
       <c r="B42" s="42"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
       <c r="E42" s="5" t="s">
         <v>397</v>
       </c>
@@ -6849,8 +7140,8 @@
     <row r="43" spans="1:7">
       <c r="A43" s="46"/>
       <c r="B43" s="43"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
       <c r="E43" s="5" t="s">
         <v>76</v>
       </c>
@@ -6871,107 +7162,903 @@
       <c r="G44" s="16"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="3"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="A45" s="44" t="s">
+        <v>408</v>
+      </c>
+      <c r="B45" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="3"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="A46" s="45"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="3"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="A47" s="45"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="3"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="A48" s="45"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="3"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="A49" s="45"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="3"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="19" t="s">
+      <c r="A50" s="45"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="45"/>
+      <c r="B51" s="42"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="45"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="21" t="s">
+        <v>419</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="45"/>
+      <c r="B53" s="42"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="45"/>
+      <c r="B54" s="42"/>
+      <c r="C54" s="21" t="s">
+        <v>423</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="45"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="45"/>
+      <c r="B56" s="42"/>
+      <c r="C56" s="21" t="s">
+        <v>426</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>427</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="17" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="45"/>
+      <c r="B57" s="42"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="45"/>
+      <c r="B58" s="42"/>
+      <c r="C58" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="45"/>
+      <c r="B59" s="42"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="45"/>
+      <c r="B60" s="42"/>
+      <c r="C60" s="21" t="s">
+        <v>432</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>433</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="17" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="45"/>
+      <c r="B61" s="42"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="45"/>
+      <c r="B62" s="42"/>
+      <c r="C62" s="21" t="s">
+        <v>435</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>436</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="45"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="45"/>
+      <c r="B64" s="42"/>
+      <c r="C64" s="21" t="s">
+        <v>439</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>440</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G64" s="17" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="45"/>
+      <c r="B65" s="42"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="45"/>
+      <c r="B66" s="42"/>
+      <c r="C66" s="21" t="s">
+        <v>443</v>
+      </c>
+      <c r="D66" s="21" t="s">
+        <v>444</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="46"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="13"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="44" t="s">
+        <v>446</v>
+      </c>
+      <c r="B69" s="41" t="s">
+        <v>447</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="45"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="45"/>
+      <c r="B71" s="42"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="45"/>
+      <c r="B72" s="42"/>
+      <c r="C72" s="21" t="s">
+        <v>395</v>
+      </c>
+      <c r="D72" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G72" s="17" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="45"/>
+      <c r="B73" s="42"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="45"/>
+      <c r="B74" s="42"/>
+      <c r="C74" s="21" t="s">
+        <v>453</v>
+      </c>
+      <c r="D74" s="21" t="s">
+        <v>455</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="45"/>
+      <c r="B75" s="42"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="46"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="13"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="3"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="3"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="3"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="3"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="3"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="3"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="3"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="3"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="3"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="3"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="3"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="3"/>
+      <c r="B85" s="18"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="3"/>
+      <c r="B86" s="18"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="3"/>
+      <c r="B87" s="18"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="3"/>
+      <c r="B88" s="18"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="3"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="3"/>
+      <c r="B90" s="18"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="3"/>
+      <c r="B91" s="18"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="3"/>
+      <c r="B92" s="18"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="3"/>
+      <c r="B93" s="18"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" s="3"/>
+      <c r="B94" s="18"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" s="3"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" s="3"/>
+      <c r="B96" s="18"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="3"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" s="3"/>
+      <c r="B98" s="18"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="3"/>
+      <c r="B99" s="18"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" s="3"/>
+      <c r="B100" s="18"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="3"/>
+      <c r="B101" s="18"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="3"/>
+      <c r="B102" s="18"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="3"/>
+      <c r="B103" s="18"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="7"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="3"/>
+      <c r="B104" s="18"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="3"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="7"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" s="3"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="3"/>
+      <c r="B107" s="18"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="3"/>
+      <c r="B108" s="18"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" s="3"/>
+      <c r="B109" s="18"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="3"/>
+      <c r="B110" s="18"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="5"/>
+      <c r="G110" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B36:B43"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="C41:C43"/>
+  <mergeCells count="58">
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D74:D76"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="B69:B76"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="B45:B67"/>
+    <mergeCell ref="A45:A67"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="A69:A76"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B2:B34"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
     <mergeCell ref="A2:A34"/>
     <mergeCell ref="D26:D28"/>
     <mergeCell ref="C26:C28"/>
@@ -6988,10 +8075,14 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B2:B34"/>
+    <mergeCell ref="B36:B43"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="C41:C43"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>